<commit_message>
Actualizado el plan de pruebas
</commit_message>
<xml_diff>
--- a/Plantilla y pruebas/Plan de Pruebas_final.xlsx
+++ b/Plantilla y pruebas/Plan de Pruebas_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alumno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blanc\TFG-RyM\Plantilla y pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D65F1C-61BE-44A8-ACB9-D9E270B29C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707EA042-6F6E-46A4-9D09-556FDD7BD36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de Pruebas" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Test Case</t>
   </si>
@@ -88,15 +88,6 @@
   </si>
   <si>
     <t>Modificar un vehiculo</t>
-  </si>
-  <si>
-    <t>Las solicitudes de usuario se visualizan correctamente</t>
-  </si>
-  <si>
-    <t>Ver las solicitudes existentes</t>
-  </si>
-  <si>
-    <t>Procesar la solicitud (Rechazada o aceptada)</t>
   </si>
   <si>
     <r>
@@ -113,6 +104,54 @@
       </rPr>
       <t>s</t>
     </r>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Se muestran los detalles</t>
+  </si>
+  <si>
+    <t>Login correcto</t>
+  </si>
+  <si>
+    <t>Los detalles del vehiculo se cargan al pulsarlo</t>
+  </si>
+  <si>
+    <t>Se cargan los coches de bbdd</t>
+  </si>
+  <si>
+    <t>Registro correcto</t>
+  </si>
+  <si>
+    <t>El usuario puede pedir cita en relacion o no a un vehiculo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se crean las citas con o sin vehiculo </t>
+  </si>
+  <si>
+    <t>El usuario puede buscar un vehiculo gracias a criterios establecidos</t>
+  </si>
+  <si>
+    <t>Se crea un vehiculo y se guarda en bbdd</t>
+  </si>
+  <si>
+    <t>Se cargan los detalles de un vehiculo con opcion de actualizar</t>
+  </si>
+  <si>
+    <t>Ver las citas existentes</t>
+  </si>
+  <si>
+    <t>Procesar la citas (Rechazada o aceptada)</t>
+  </si>
+  <si>
+    <t>Se visualizan las citas que han hecho los usuarios</t>
+  </si>
+  <si>
+    <t>Se marcan como rechazadas o aceptadas (si se aceptan y tienen vehiculo relacionado, se crea una venta)</t>
+  </si>
+  <si>
+    <t>Se muestran los usuarios con opcion de actualizarlos</t>
   </si>
 </sst>
 </file>
@@ -150,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,8 +214,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -236,34 +281,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,21 +625,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="1"/>
+    <col min="6" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -581,7 +659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -594,13 +672,15 @@
       <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
       <c r="B3" s="5">
         <v>2</v>
       </c>
@@ -610,13 +690,15 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
       <c r="B4" s="5">
         <v>3</v>
       </c>
@@ -626,54 +708,67 @@
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
       <c r="B5" s="5">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
       <c r="B6" s="5">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
       <c r="B7" s="5">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="12"/>
       <c r="B8" s="5">
         <v>7</v>
       </c>
@@ -686,8 +781,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="5">
@@ -696,64 +791,85 @@
       <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
       <c r="B10" s="5">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
       <c r="B11" s="5">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="1">
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="2">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="1">
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="7">
         <v>12</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>24</v>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A9:A13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se muestran las ventas que hay en bbdd
</commit_message>
<xml_diff>
--- a/Plantilla y pruebas/Plan de Pruebas_final.xlsx
+++ b/Plantilla y pruebas/Plan de Pruebas_final.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blanc\TFG-RyM\Plantilla y pruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miguel_blanco\Desktop\TFG-RyM\Plantilla y pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707EA042-6F6E-46A4-9D09-556FDD7BD36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="598"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de Pruebas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Test Case</t>
   </si>
@@ -153,11 +152,14 @@
   <si>
     <t>Se muestran los usuarios con opcion de actualizarlos</t>
   </si>
+  <si>
+    <t>Medio OK</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -189,7 +191,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,8 +222,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -282,17 +290,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -301,15 +298,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -324,14 +312,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -340,9 +325,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,24 +606,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.6640625" style="1"/>
+    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -659,8 +644,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="5">
@@ -679,8 +664,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
       <c r="B3" s="5">
         <v>2</v>
       </c>
@@ -697,8 +682,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
       <c r="B4" s="5">
         <v>3</v>
       </c>
@@ -715,8 +700,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
       <c r="B5" s="5">
         <v>4</v>
       </c>
@@ -729,12 +714,12 @@
       <c r="E5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
+      <c r="F5" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
       <c r="B6" s="5">
         <v>5</v>
       </c>
@@ -747,12 +732,12 @@
       <c r="E6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
+      <c r="F6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
       <c r="B7" s="5">
         <v>6</v>
       </c>
@@ -767,8 +752,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
       <c r="B8" s="5">
         <v>7</v>
       </c>
@@ -781,7 +766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
@@ -795,11 +780,11 @@
         <v>31</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F9" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="5">
         <v>9</v>
@@ -811,11 +796,11 @@
         <v>32</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="5">
         <v>10</v>
@@ -827,11 +812,11 @@
         <v>35</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F11" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="2">
         <v>11</v>
@@ -839,7 +824,7 @@
       <c r="C12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E12" s="2"/>
@@ -847,8 +832,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
       <c r="B13" s="7">
         <v>12</v>
       </c>
@@ -859,8 +844,8 @@
         <v>37</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="4" t="s">
-        <v>5</v>
+      <c r="F13" s="13" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizado el plan de pruebas, todas las pruebas de la app OK
</commit_message>
<xml_diff>
--- a/Plantilla y pruebas/Plan de Pruebas_final.xlsx
+++ b/Plantilla y pruebas/Plan de Pruebas_final.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miguel_blanco\Desktop\TFG-RyM\Plantilla y pruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blanc\TFG-RyM\Plantilla y pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0553B648-5E25-4D54-85FF-A7FA45467552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="598"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de Pruebas" sheetId="1" r:id="rId1"/>
@@ -159,7 +160,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -316,6 +317,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -325,8 +328,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,25 +607,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7109375" style="1"/>
+    <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -644,8 +645,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="5">
@@ -664,8 +665,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
       <c r="B3" s="5">
         <v>2</v>
       </c>
@@ -682,8 +683,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="12"/>
       <c r="B4" s="5">
         <v>3</v>
       </c>
@@ -700,8 +701,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="12"/>
       <c r="B5" s="5">
         <v>4</v>
       </c>
@@ -714,12 +715,12 @@
       <c r="E5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="12"/>
       <c r="B6" s="5">
         <v>5</v>
       </c>
@@ -736,8 +737,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="12"/>
       <c r="B7" s="5">
         <v>6</v>
       </c>
@@ -752,8 +753,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
       <c r="B8" s="5">
         <v>7</v>
       </c>
@@ -766,8 +767,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="5">
@@ -784,8 +785,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="12"/>
       <c r="B10" s="5">
         <v>9</v>
       </c>
@@ -800,8 +801,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="12"/>
       <c r="B11" s="5">
         <v>10</v>
       </c>
@@ -816,8 +817,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="12"/>
       <c r="B12" s="2">
         <v>11</v>
       </c>
@@ -828,12 +829,12 @@
         <v>36</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="F12" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
       <c r="B13" s="7">
         <v>12</v>
       </c>
@@ -844,7 +845,7 @@
         <v>37</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="10" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>